<commit_message>
updated game with animations & goals
</commit_message>
<xml_diff>
--- a/tableconfiguration.xlsx
+++ b/tableconfiguration.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhilashakumar/helping-behavior-game/games/helping-game/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhilashakumar/bigger-helptown/games/helping-game-bigger/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACEBD26-21BC-C64E-9E9F-8C309CEA1367}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A4921A-66D7-1044-B37C-F4419E39DA8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{BC9B4203-94A0-5243-8CBD-CB7149E0043F}"/>
+    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15600" xr2:uid="{3E058163-EEE8-FE47-92DF-6C27D6D7F5A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,15 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>A1</t>
   </si>
   <si>
     <t>A2</t>
-  </si>
-  <si>
-    <t>A3</t>
   </si>
   <si>
     <t>B1</t>
@@ -51,25 +48,10 @@
     <t>B2</t>
   </si>
   <si>
-    <t>B3</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
     <t>C2</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>B4</t>
-  </si>
-  <si>
-    <t>C4</t>
   </si>
 </sst>
 </file>
@@ -85,15 +67,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -110,16 +110,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -435,171 +477,616 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0975BE81-E6DB-F548-9CE7-2B11D2DA96F1}">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6715F407-1D89-524D-9AFB-2AF3A682D1DE}">
+  <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="1">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" s="9">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="9">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="2">
         <v>2</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="10">
         <v>3</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="9">
         <v>4</v>
       </c>
-      <c r="F1" s="1">
+      <c r="F1" s="2">
         <v>5</v>
       </c>
-      <c r="G1" s="1">
+      <c r="G1" s="10">
         <v>6</v>
       </c>
-      <c r="H1" s="2">
+      <c r="H1" s="9">
         <v>7</v>
       </c>
-      <c r="I1" s="1">
+      <c r="I1" s="2">
         <v>8</v>
       </c>
-      <c r="J1" s="1">
+      <c r="J1" s="10">
         <v>9</v>
       </c>
-      <c r="K1" s="1">
+      <c r="K1" s="9">
         <v>10</v>
       </c>
-      <c r="L1" s="1">
+      <c r="L1" s="2">
         <v>11</v>
       </c>
+      <c r="M1" s="10">
+        <v>12</v>
+      </c>
+      <c r="N1" s="9">
+        <v>13</v>
+      </c>
+      <c r="O1" s="2">
+        <v>14</v>
+      </c>
+      <c r="P1" s="10">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="9">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>12</v>
-      </c>
-      <c r="B2" s="1">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1">
-        <v>14</v>
-      </c>
-      <c r="D2" s="2">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1">
-        <v>16</v>
-      </c>
-      <c r="F2" s="1">
-        <v>17</v>
-      </c>
-      <c r="G2" s="1">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" s="9">
         <v>18</v>
       </c>
-      <c r="H2" s="2">
+      <c r="B2" s="9">
         <v>19</v>
       </c>
-      <c r="I2" s="1">
+      <c r="C2" s="2">
         <v>20</v>
       </c>
-      <c r="J2" s="1">
+      <c r="D2" s="10">
         <v>21</v>
       </c>
-      <c r="K2" s="1">
+      <c r="E2" s="9">
         <v>22</v>
       </c>
-      <c r="L2" s="1">
+      <c r="F2" s="2">
         <v>23</v>
       </c>
+      <c r="G2" s="10">
+        <v>24</v>
+      </c>
+      <c r="H2" s="9">
+        <v>25</v>
+      </c>
+      <c r="I2" s="2">
+        <v>26</v>
+      </c>
+      <c r="J2" s="10">
+        <v>27</v>
+      </c>
+      <c r="K2" s="9">
+        <v>28</v>
+      </c>
+      <c r="L2" s="2">
+        <v>29</v>
+      </c>
+      <c r="M2" s="10">
+        <v>30</v>
+      </c>
+      <c r="N2" s="9">
+        <v>31</v>
+      </c>
+      <c r="O2" s="2">
+        <v>32</v>
+      </c>
+      <c r="P2" s="10">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="9">
+        <v>34</v>
+      </c>
+      <c r="R2" s="2">
+        <v>35</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>24</v>
-      </c>
-      <c r="B3" s="1">
-        <v>25</v>
-      </c>
-      <c r="C3" s="1">
-        <v>26</v>
-      </c>
-      <c r="D3" s="2">
-        <v>27</v>
-      </c>
-      <c r="E3" s="1">
-        <v>28</v>
-      </c>
-      <c r="F3" s="1">
-        <v>29</v>
-      </c>
-      <c r="G3" s="1">
-        <v>30</v>
-      </c>
-      <c r="H3" s="2">
-        <v>31</v>
-      </c>
-      <c r="I3" s="1">
-        <v>32</v>
-      </c>
-      <c r="J3" s="1">
-        <v>33</v>
-      </c>
-      <c r="K3" s="1">
-        <v>34</v>
-      </c>
-      <c r="L3" s="1">
-        <v>35</v>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="9">
+        <v>36</v>
+      </c>
+      <c r="B3" s="9">
+        <v>37</v>
+      </c>
+      <c r="C3" s="2">
+        <v>38</v>
+      </c>
+      <c r="D3" s="10">
+        <v>39</v>
+      </c>
+      <c r="E3" s="9">
+        <v>40</v>
+      </c>
+      <c r="F3" s="2">
+        <v>41</v>
+      </c>
+      <c r="G3" s="10">
+        <v>42</v>
+      </c>
+      <c r="H3" s="9">
+        <v>43</v>
+      </c>
+      <c r="I3" s="2">
+        <v>44</v>
+      </c>
+      <c r="J3" s="10">
+        <v>45</v>
+      </c>
+      <c r="K3" s="9">
+        <v>46</v>
+      </c>
+      <c r="L3" s="2">
+        <v>47</v>
+      </c>
+      <c r="M3" s="10">
+        <v>48</v>
+      </c>
+      <c r="N3" s="9">
+        <v>49</v>
+      </c>
+      <c r="O3" s="2">
+        <v>50</v>
+      </c>
+      <c r="P3" s="10">
+        <v>51</v>
+      </c>
+      <c r="Q3" s="9">
+        <v>52</v>
+      </c>
+      <c r="R3" s="2">
+        <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="9">
+        <v>54</v>
+      </c>
+      <c r="B4" s="9">
+        <v>55</v>
+      </c>
+      <c r="C4" s="2">
+        <v>56</v>
+      </c>
+      <c r="D4" s="10">
+        <v>57</v>
+      </c>
+      <c r="E4" s="9">
+        <v>58</v>
+      </c>
+      <c r="F4" s="2">
+        <v>59</v>
+      </c>
+      <c r="G4" s="10">
+        <v>60</v>
+      </c>
+      <c r="H4" s="9">
+        <v>61</v>
+      </c>
+      <c r="I4" s="2">
+        <v>62</v>
+      </c>
+      <c r="J4" s="10">
+        <v>63</v>
+      </c>
+      <c r="K4" s="9">
+        <v>64</v>
+      </c>
+      <c r="L4" s="2">
+        <v>65</v>
+      </c>
+      <c r="M4" s="10">
+        <v>66</v>
+      </c>
+      <c r="N4" s="9">
+        <v>67</v>
+      </c>
+      <c r="O4" s="2">
+        <v>68</v>
+      </c>
+      <c r="P4" s="10">
+        <v>69</v>
+      </c>
+      <c r="Q4" s="9">
+        <v>70</v>
+      </c>
+      <c r="R4" s="2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="9">
+        <v>72</v>
+      </c>
+      <c r="B5" s="9">
+        <v>73</v>
+      </c>
+      <c r="C5" s="2">
+        <v>74</v>
+      </c>
+      <c r="D5" s="10">
+        <v>75</v>
+      </c>
+      <c r="E5" s="9">
+        <v>76</v>
+      </c>
+      <c r="F5" s="2">
+        <v>77</v>
+      </c>
+      <c r="G5" s="10">
+        <v>78</v>
+      </c>
+      <c r="H5" s="9">
+        <v>79</v>
+      </c>
+      <c r="I5" s="2">
+        <v>80</v>
+      </c>
+      <c r="J5" s="10">
+        <v>81</v>
+      </c>
+      <c r="K5" s="9">
+        <v>82</v>
+      </c>
+      <c r="L5" s="2">
+        <v>83</v>
+      </c>
+      <c r="M5" s="10">
+        <v>84</v>
+      </c>
+      <c r="N5" s="9">
+        <v>85</v>
+      </c>
+      <c r="O5" s="2">
+        <v>86</v>
+      </c>
+      <c r="P5" s="10">
+        <v>87</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>88</v>
+      </c>
+      <c r="R5" s="2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="9">
+        <v>90</v>
+      </c>
+      <c r="B6" s="9">
+        <v>91</v>
+      </c>
+      <c r="C6" s="2">
+        <v>92</v>
+      </c>
+      <c r="D6" s="10">
+        <v>93</v>
+      </c>
+      <c r="E6" s="9">
+        <v>94</v>
+      </c>
+      <c r="F6" s="2">
+        <v>95</v>
+      </c>
+      <c r="G6" s="10">
+        <v>96</v>
+      </c>
+      <c r="H6" s="9">
+        <v>97</v>
+      </c>
+      <c r="I6" s="2">
+        <v>98</v>
+      </c>
+      <c r="J6" s="10">
+        <v>99</v>
+      </c>
+      <c r="K6" s="9">
+        <v>100</v>
+      </c>
+      <c r="L6" s="2">
+        <v>101</v>
+      </c>
+      <c r="M6" s="10">
+        <v>102</v>
+      </c>
+      <c r="N6" s="9">
+        <v>103</v>
+      </c>
+      <c r="O6" s="2">
+        <v>104</v>
+      </c>
+      <c r="P6" s="10">
+        <v>105</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>106</v>
+      </c>
+      <c r="R6" s="2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E7" s="7"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="H7" s="8"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="K7" s="8"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="N7" s="11"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>11</v>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="13"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>108</v>
+      </c>
+      <c r="B12" s="1">
+        <v>109</v>
+      </c>
+      <c r="C12" s="2">
+        <v>110</v>
+      </c>
+      <c r="D12" s="2">
+        <v>111</v>
+      </c>
+      <c r="E12" s="1">
+        <v>112</v>
+      </c>
+      <c r="F12" s="1">
+        <v>113</v>
+      </c>
+      <c r="G12" s="1">
+        <v>114</v>
+      </c>
+      <c r="H12" s="2">
+        <v>115</v>
+      </c>
+      <c r="I12" s="1">
+        <v>116</v>
+      </c>
+      <c r="J12" s="1">
+        <v>117</v>
+      </c>
+      <c r="K12" s="1">
+        <v>118</v>
+      </c>
+      <c r="L12" s="1">
+        <v>119</v>
+      </c>
+      <c r="M12" s="1">
+        <v>120</v>
+      </c>
+      <c r="N12" s="1">
+        <v>121</v>
+      </c>
+      <c r="O12" s="1">
+        <v>122</v>
+      </c>
+      <c r="P12" s="1">
+        <v>123</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>124</v>
+      </c>
+      <c r="R12" s="1">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>126</v>
+      </c>
+      <c r="B13" s="1">
+        <v>127</v>
+      </c>
+      <c r="C13" s="2">
+        <v>128</v>
+      </c>
+      <c r="D13" s="1">
+        <v>129</v>
+      </c>
+      <c r="E13" s="1">
+        <v>130</v>
+      </c>
+      <c r="F13" s="1">
+        <v>131</v>
+      </c>
+      <c r="G13" s="1">
+        <v>132</v>
+      </c>
+      <c r="H13" s="1">
+        <v>133</v>
+      </c>
+      <c r="I13" s="1">
+        <v>134</v>
+      </c>
+      <c r="J13" s="1">
+        <v>135</v>
+      </c>
+      <c r="K13" s="1">
+        <v>136</v>
+      </c>
+      <c r="L13" s="1">
+        <v>137</v>
+      </c>
+      <c r="M13" s="1">
+        <v>138</v>
+      </c>
+      <c r="N13" s="1">
+        <v>139</v>
+      </c>
+      <c r="O13" s="1">
+        <v>140</v>
+      </c>
+      <c r="P13" s="1">
+        <v>141</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>142</v>
+      </c>
+      <c r="R13" s="1">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>144</v>
+      </c>
+      <c r="B14" s="1">
+        <v>145</v>
+      </c>
+      <c r="C14" s="2">
+        <v>146</v>
+      </c>
+      <c r="D14" s="2">
+        <v>147</v>
+      </c>
+      <c r="E14" s="1">
+        <v>148</v>
+      </c>
+      <c r="F14" s="1">
+        <v>149</v>
+      </c>
+      <c r="G14" s="1">
+        <v>150</v>
+      </c>
+      <c r="H14" s="2">
+        <v>151</v>
+      </c>
+      <c r="I14" s="1">
+        <v>152</v>
+      </c>
+      <c r="J14" s="1">
+        <v>153</v>
+      </c>
+      <c r="K14" s="1">
+        <v>154</v>
+      </c>
+      <c r="L14" s="1">
+        <v>155</v>
+      </c>
+      <c r="M14" s="1">
+        <v>156</v>
+      </c>
+      <c r="N14" s="1">
+        <v>157</v>
+      </c>
+      <c r="O14" s="1">
+        <v>158</v>
+      </c>
+      <c r="P14" s="1">
+        <v>159</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>160</v>
+      </c>
+      <c r="R14" s="1">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>162</v>
+      </c>
+      <c r="B15" s="1">
+        <v>163</v>
+      </c>
+      <c r="C15" s="2">
+        <v>164</v>
+      </c>
+      <c r="D15" s="1">
+        <v>165</v>
+      </c>
+      <c r="E15" s="1">
+        <v>166</v>
+      </c>
+      <c r="F15" s="1">
+        <v>167</v>
+      </c>
+      <c r="G15" s="1">
+        <v>168</v>
+      </c>
+      <c r="H15" s="1">
+        <v>169</v>
+      </c>
+      <c r="I15" s="1">
+        <v>170</v>
+      </c>
+      <c r="J15" s="1">
+        <v>171</v>
+      </c>
+      <c r="K15" s="1">
+        <v>172</v>
+      </c>
+      <c r="L15" s="1">
+        <v>173</v>
+      </c>
+      <c r="M15" s="1">
+        <v>174</v>
+      </c>
+      <c r="N15" s="1">
+        <v>175</v>
+      </c>
+      <c r="O15" s="1">
+        <v>176</v>
+      </c>
+      <c r="P15" s="1">
+        <v>177</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>178</v>
+      </c>
+      <c r="R15" s="1">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:I7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>